<commit_message>
Actualización escaleta con observaciones 16/10/15
Actualización escaleta con observaciones de recursos greco
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion03/CS_08_03_CO_Escaleta.xlsx
+++ b/fuentes/contenidos/grado08/guion03/CS_08_03_CO_Escaleta.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="242">
   <si>
     <t>Asignatura</t>
   </si>
@@ -674,9 +674,6 @@
     <t>Recurso M101AP-01</t>
   </si>
   <si>
-    <t>Recuerda qué fue el Grito de independencia</t>
-  </si>
-  <si>
     <t>Conoce la lucha de Nariño contra el federalismo</t>
   </si>
   <si>
@@ -717,6 +714,30 @@
   </si>
   <si>
     <t>Presentación que expone las exigencias de los comuneros frente a la aplicación de las Reformas borbónicas</t>
+  </si>
+  <si>
+    <t>Comprende el Memorial de agravios</t>
+  </si>
+  <si>
+    <t>Recuerda la guerra de los Conventillos</t>
+  </si>
+  <si>
+    <t>Actividad que permite sitetizar aspectos generales de la guerra de los Conventillos</t>
+  </si>
+  <si>
+    <t>Recuerda la guerra de los Supremos</t>
+  </si>
+  <si>
+    <t>Actividad para identificar los apellidos de personajes relacionados con la guerra de los Supremos</t>
+  </si>
+  <si>
+    <t>Interactivo que permite reflexionar sobre el sufragio universal en las constituciones políticas de la Patria Boba, la Gran Colombia y la República de la Nueva Granada</t>
+  </si>
+  <si>
+    <t>Actividades sobre la República de la Nueva Granada (1839-1858)</t>
+  </si>
+  <si>
+    <t>Montado y editado en greco por Nathalia.</t>
   </si>
   <si>
     <r>
@@ -743,31 +764,13 @@
     </r>
   </si>
   <si>
-    <t>Comprende el Memorial de agravios</t>
-  </si>
-  <si>
-    <t>Recuerda la guerra de los Conventillos</t>
-  </si>
-  <si>
-    <t>Actividad que permite sitetizar aspectos generales de la guerra de los Conventillos</t>
-  </si>
-  <si>
-    <t>Recuerda la guerra de los Supremos</t>
-  </si>
-  <si>
-    <t>Actividad para identificar los apellidos de personajes relacionados con la guerra de los Supremos</t>
-  </si>
-  <si>
-    <t>Interactivo que permite reflexionar sobre el sufragio universal en las constituciones políticas de la Patria Boba, la Gran Colombia y la República de la Nueva Granada</t>
-  </si>
-  <si>
-    <t>Actividades sobre la República de la Nueva Granada (1839-1858)</t>
-  </si>
-  <si>
-    <t>Montado y editado en greco por Nathalia.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asignado a Ana Hoyos para autoría. </t>
+    <t>Asignado a Ana Hoyos para autoría. Editado en greco por Nathalia.</t>
+  </si>
+  <si>
+    <t>Recuerda qué fue el grito de Independencia</t>
+  </si>
+  <si>
+    <t>Asignado a Ana Hoyos para autoría.  Editado en greco por Nathalia.</t>
   </si>
 </sst>
 </file>
@@ -1500,9 +1503,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U284"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O13" sqref="O13"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T18" sqref="T18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1628,7 +1631,7 @@
         <v>122</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>123</v>
@@ -1649,7 +1652,7 @@
         <v>19</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="K3" s="11" t="s">
         <v>20</v>
@@ -1689,7 +1692,7 @@
         <v>122</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D4" s="18" t="s">
         <v>123</v>
@@ -1710,7 +1713,7 @@
         <v>20</v>
       </c>
       <c r="J4" s="38" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
       <c r="K4" s="23" t="s">
         <v>20</v>
@@ -1722,8 +1725,8 @@
       <c r="N4" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="O4" s="19" t="s">
-        <v>240</v>
+      <c r="O4" s="30" t="s">
+        <v>239</v>
       </c>
       <c r="P4" s="19" t="s">
         <v>19</v>
@@ -1752,7 +1755,7 @@
         <v>122</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D5" s="18" t="s">
         <v>123</v>
@@ -1773,7 +1776,7 @@
         <v>20</v>
       </c>
       <c r="J5" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K5" s="23" t="s">
         <v>20</v>
@@ -1786,7 +1789,7 @@
         <v>28</v>
       </c>
       <c r="O5" s="19" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="P5" s="19" t="s">
         <v>19</v>
@@ -1815,7 +1818,7 @@
         <v>122</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D6" s="18" t="s">
         <v>123</v>
@@ -1849,7 +1852,7 @@
         <v>121</v>
       </c>
       <c r="O6" s="19" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="P6" s="19" t="s">
         <v>20</v>
@@ -1878,7 +1881,7 @@
         <v>122</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D7" s="18" t="s">
         <v>123</v>
@@ -1887,10 +1890,10 @@
         <v>126</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H7" s="19">
         <v>5</v>
@@ -1912,7 +1915,7 @@
         <v>36</v>
       </c>
       <c r="O7" s="19" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="P7" s="19" t="s">
         <v>20</v>
@@ -1941,7 +1944,7 @@
         <v>122</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D8" s="18" t="s">
         <v>123</v>
@@ -1978,7 +1981,7 @@
         <v>122</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>123</v>
@@ -1990,7 +1993,7 @@
         <v>134</v>
       </c>
       <c r="G9" s="37" t="s">
-        <v>216</v>
+        <v>240</v>
       </c>
       <c r="H9" s="19">
         <v>6</v>
@@ -2011,8 +2014,8 @@
       <c r="N9" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="O9" s="19" t="s">
-        <v>240</v>
+      <c r="O9" s="30" t="s">
+        <v>241</v>
       </c>
       <c r="P9" s="19" t="s">
         <v>19</v>
@@ -2041,7 +2044,7 @@
         <v>122</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D10" s="18" t="s">
         <v>123</v>
@@ -2053,7 +2056,7 @@
         <v>137</v>
       </c>
       <c r="G10" s="37" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H10" s="19">
         <v>7</v>
@@ -2075,7 +2078,7 @@
         <v>36</v>
       </c>
       <c r="O10" s="19" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="P10" s="19" t="s">
         <v>19</v>
@@ -2104,7 +2107,7 @@
         <v>122</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D11" s="18" t="s">
         <v>123</v>
@@ -2165,7 +2168,7 @@
         <v>122</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D12" s="18" t="s">
         <v>123</v>
@@ -2198,8 +2201,8 @@
       <c r="N12" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="O12" s="19" t="s">
-        <v>240</v>
+      <c r="O12" s="30" t="s">
+        <v>239</v>
       </c>
       <c r="P12" s="19" t="s">
         <v>19</v>
@@ -2228,7 +2231,7 @@
         <v>122</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D13" s="18" t="s">
         <v>123</v>
@@ -2265,7 +2268,7 @@
         <v>122</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D14" s="18" t="s">
         <v>123</v>
@@ -2312,7 +2315,7 @@
         <v>198</v>
       </c>
       <c r="T14" s="52" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="U14" s="50" t="s">
         <v>199</v>
@@ -2326,7 +2329,7 @@
         <v>122</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D15" s="18" t="s">
         <v>123</v>
@@ -2357,7 +2360,9 @@
       <c r="N15" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="O15" s="19"/>
+      <c r="O15" s="19" t="s">
+        <v>237</v>
+      </c>
       <c r="P15" s="19" t="s">
         <v>19</v>
       </c>
@@ -2385,7 +2390,7 @@
         <v>122</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D16" s="18" t="s">
         <v>123</v>
@@ -2444,7 +2449,7 @@
         <v>122</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D17" s="18" t="s">
         <v>154</v>
@@ -2479,7 +2484,7 @@
         <v>122</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D18" s="18" t="s">
         <v>154</v>
@@ -2538,7 +2543,7 @@
         <v>122</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D19" s="18" t="s">
         <v>154</v>
@@ -2597,13 +2602,13 @@
         <v>122</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D20" s="18" t="s">
         <v>160</v>
       </c>
       <c r="E20" s="39" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F20" s="19"/>
       <c r="G20" s="20"/>
@@ -2632,19 +2637,19 @@
         <v>122</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D21" s="18" t="s">
         <v>160</v>
       </c>
       <c r="E21" s="39" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G21" s="20" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="H21" s="19">
         <v>15</v>
@@ -2653,7 +2658,7 @@
         <v>20</v>
       </c>
       <c r="J21" s="22" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="K21" s="23" t="s">
         <v>20</v>
@@ -2693,16 +2698,16 @@
         <v>122</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D22" s="18" t="s">
         <v>160</v>
       </c>
       <c r="E22" s="39" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F22" s="19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G22" s="20"/>
       <c r="H22" s="19"/>
@@ -2730,19 +2735,19 @@
         <v>122</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D23" s="18" t="s">
         <v>160</v>
       </c>
       <c r="E23" s="39" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F23" s="30" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G23" s="20" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="H23" s="19">
         <v>16</v>
@@ -2751,7 +2756,7 @@
         <v>20</v>
       </c>
       <c r="J23" s="22" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="K23" s="23" t="s">
         <v>20</v>
@@ -2764,7 +2769,7 @@
         <v>51</v>
       </c>
       <c r="O23" s="19" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="P23" s="19" t="s">
         <v>20</v>
@@ -2793,7 +2798,7 @@
         <v>122</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D24" s="18" t="s">
         <v>160</v>
@@ -2828,7 +2833,7 @@
         <v>122</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D25" s="18" t="s">
         <v>160</v>
@@ -2887,7 +2892,7 @@
         <v>122</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D26" s="18" t="s">
         <v>160</v>
@@ -2932,7 +2937,7 @@
         <v>198</v>
       </c>
       <c r="T26" s="52" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="U26" s="50" t="s">
         <v>199</v>
@@ -2946,7 +2951,7 @@
         <v>122</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D27" s="18" t="s">
         <v>160</v>
@@ -2981,7 +2986,7 @@
         <v>122</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D28" s="18" t="s">
         <v>160</v>
@@ -3000,7 +3005,7 @@
         <v>19</v>
       </c>
       <c r="J28" s="38" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K28" s="23" t="s">
         <v>20</v>
@@ -3040,7 +3045,7 @@
         <v>122</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D29" s="18" t="s">
         <v>160</v>
@@ -3099,7 +3104,7 @@
         <v>122</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D30" s="18" t="s">
         <v>160</v>
@@ -3118,7 +3123,7 @@
         <v>20</v>
       </c>
       <c r="J30" s="29" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="K30" s="23" t="s">
         <v>20</v>
@@ -3158,7 +3163,7 @@
         <v>122</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D31" s="18" t="s">
         <v>174</v>
@@ -3215,7 +3220,7 @@
         <v>122</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D32" s="18" t="s">
         <v>174</v>
@@ -3272,7 +3277,7 @@
         <v>122</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D33" s="18" t="s">
         <v>179</v>
@@ -3289,7 +3294,7 @@
         <v>20</v>
       </c>
       <c r="J33" s="22" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K33" s="23" t="s">
         <v>20</v>
@@ -3317,7 +3322,7 @@
         <v>122</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D34" s="18" t="s">
         <v>179</v>
@@ -3334,7 +3339,7 @@
         <v>20</v>
       </c>
       <c r="J34" s="22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K34" s="23" t="s">
         <v>20</v>
@@ -3374,7 +3379,7 @@
         <v>122</v>
       </c>
       <c r="C35" s="41" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D35" s="18" t="s">
         <v>179</v>

</xml_diff>